<commit_message>
The Weak Attack Update
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3090845e3ab6f0a2/01.Cesun/2025/25-2/Frontend/Semana 7/HackAndSlash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD2279FF-1D1C-41B3-B808-0DA2BAB5470E}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_AD4D2F04E46CFB4ACB3E203F1597FE22683EDF0C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECD3E5F7-4965-437C-83DC-ED3762DDFFB7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +443,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>

</xml_diff>